<commit_message>
i think everything is fixed and working now.
</commit_message>
<xml_diff>
--- a/WORK/prices workbook2.xlsx
+++ b/WORK/prices workbook2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ACS\Dev-5\WORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BAEAA2B-4535-40CB-9D4F-80078E0A5095}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F46C86-78F9-4720-A3FD-29737A4FF58D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10393" yWindow="2353" windowWidth="15207" windowHeight="10660" activeTab="1" xr2:uid="{206A8742-963A-4C00-9A73-033B15878E20}"/>
+    <workbookView xWindow="33" yWindow="0" windowWidth="11187" windowHeight="6400" activeTab="1" xr2:uid="{206A8742-963A-4C00-9A73-033B15878E20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -9222,12 +9222,70 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DC3F49-683E-4A09-84CB-EE52AA9ECA73}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A1">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A5">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A6">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A7">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A8">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A9">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A10">
+        <f>SUM(A1:A9)</f>
+        <v>20.330000000000002</v>
+      </c>
+      <c r="B10">
+        <f>A10*75</f>
+        <v>1524.7500000000002</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>